<commit_message>
simplify cell data example. * CellDataComposer do not extends AbstractDemoComposer at all and modify related codes.
</commit_message>
<xml_diff>
--- a/zssessentials/src/main/webapp/WEB-INF/books/blank.xlsx
+++ b/zssessentials/src/main/webapp/WEB-INF/books/blank.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="17040" windowHeight="11280" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="345" windowWidth="17040" windowHeight="11280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20,14 +24,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -355,14 +359,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -370,11 +378,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+  </cols>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>